<commit_message>
Replace in example department report
</commit_message>
<xml_diff>
--- a/documentation/example_dept_report/test_risk_report_202311.xlsx
+++ b/documentation/example_dept_report/test_risk_report_202311.xlsx
@@ -1,19 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amhan\Documents\GitHub\format-report\documentation\example_dept_report\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29ECD2E2-434E-4EF4-A17D-63690F07B034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="AIP Risk Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Department Risk Levels" sheetId="2" r:id="rId2"/>
-    <sheet name="Collection Risk Levels" sheetId="3" r:id="rId3"/>
-    <sheet name="AIP Risk Levels" sheetId="4" r:id="rId4"/>
+    <sheet name="AIP_Risk_Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Department_Risk_Levels" sheetId="2" r:id="rId2"/>
+    <sheet name="Collection_Risk_Levels" sheetId="3" r:id="rId3"/>
+    <sheet name="AIP_Risk_Levels" sheetId="4" r:id="rId4"/>
     <sheet name="Formats" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -236,18 +242,6 @@
     <t>Formats</t>
   </si>
   <si>
-    <t>No Match %</t>
-  </si>
-  <si>
-    <t>High Risk %</t>
-  </si>
-  <si>
-    <t>Moderate Risk %</t>
-  </si>
-  <si>
-    <t>Low Risk %</t>
-  </si>
-  <si>
     <t>Format</t>
   </si>
   <si>
@@ -303,13 +297,25 @@
   </si>
   <si>
     <t>Plain text (Low Risk)</t>
+  </si>
+  <si>
+    <t>No_Match_%</t>
+  </si>
+  <si>
+    <t>High_Risk_%</t>
+  </si>
+  <si>
+    <t>Moderate_Risk_%</t>
+  </si>
+  <si>
+    <t>Low_Risk_%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -372,12 +378,15 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -385,13 +394,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -429,7 +446,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -463,6 +480,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -497,9 +515,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -672,14 +691,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -711,7 +742,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -743,7 +774,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -775,7 +806,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -807,7 +838,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -839,7 +870,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -871,7 +902,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -903,7 +934,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -935,7 +966,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -967,7 +998,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -999,7 +1030,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1031,7 +1062,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1063,7 +1094,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1095,7 +1126,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1127,7 +1158,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1159,7 +1190,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -1191,7 +1222,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -1223,7 +1254,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -1255,7 +1286,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -1287,7 +1318,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -1319,7 +1350,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1351,7 +1382,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -1383,7 +1414,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -1415,7 +1446,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -1447,7 +1478,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -1479,7 +1510,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -1505,7 +1536,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -1534,7 +1565,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -1566,7 +1597,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -1598,7 +1629,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -1630,7 +1661,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -1659,7 +1690,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -1688,7 +1719,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -1720,7 +1751,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -1752,7 +1783,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -1781,7 +1812,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -1813,7 +1844,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -1845,7 +1876,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>10</v>
       </c>
@@ -1877,7 +1908,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -1906,7 +1937,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>10</v>
       </c>
@@ -1937,47 +1968,55 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3" r:id="rId2"/>
-    <hyperlink ref="F4" r:id="rId3"/>
-    <hyperlink ref="F5" r:id="rId4"/>
-    <hyperlink ref="F6" r:id="rId5"/>
-    <hyperlink ref="F7" r:id="rId6"/>
-    <hyperlink ref="F8" r:id="rId7"/>
-    <hyperlink ref="F9" r:id="rId8"/>
-    <hyperlink ref="F10" r:id="rId9"/>
-    <hyperlink ref="F11" r:id="rId10"/>
-    <hyperlink ref="F12" r:id="rId11"/>
-    <hyperlink ref="F13" r:id="rId12"/>
-    <hyperlink ref="F14" r:id="rId13"/>
-    <hyperlink ref="F15" r:id="rId14"/>
-    <hyperlink ref="F16" r:id="rId15"/>
-    <hyperlink ref="F17" r:id="rId16"/>
-    <hyperlink ref="F18" r:id="rId17"/>
-    <hyperlink ref="F19" r:id="rId18"/>
-    <hyperlink ref="F20" r:id="rId19"/>
-    <hyperlink ref="F21" r:id="rId20"/>
-    <hyperlink ref="F22" r:id="rId21"/>
-    <hyperlink ref="F26" r:id="rId22"/>
-    <hyperlink ref="F28" r:id="rId23"/>
-    <hyperlink ref="F29" r:id="rId24"/>
-    <hyperlink ref="F33" r:id="rId25"/>
-    <hyperlink ref="F36" r:id="rId26"/>
-    <hyperlink ref="F37" r:id="rId27"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="F8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="F9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="F10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="F11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="F12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="F13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="F14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="F15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="F16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="F17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="F18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="F19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="F20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="F21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="F22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="F26" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="F28" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="F29" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="F33" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="F36" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="F37" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1985,19 +2024,19 @@
         <v>71</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>74</v>
+        <v>93</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -2023,14 +2062,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2038,19 +2085,19 @@
         <v>71</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>74</v>
+        <v>93</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -2070,7 +2117,7 @@
         <v>72.73</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -2090,7 +2137,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -2116,14 +2163,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2131,19 +2186,19 @@
         <v>71</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>74</v>
+        <v>93</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -2163,7 +2218,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -2183,7 +2238,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -2203,7 +2258,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -2223,7 +2278,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -2243,7 +2298,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -2263,7 +2318,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -2283,7 +2338,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -2303,7 +2358,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -2323,7 +2378,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
@@ -2343,7 +2398,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
@@ -2363,7 +2418,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
@@ -2383,7 +2438,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
@@ -2403,7 +2458,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
@@ -2423,7 +2478,7 @@
         <v>33.33</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
@@ -2449,125 +2504,144 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:T19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="59.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="46.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-    </row>
-    <row r="2" spans="1:20">
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1" t="s">
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-    </row>
-    <row r="3" spans="1:20">
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="Q3" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20">
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -2575,8 +2649,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -2637,8 +2711,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
-      <c r="A6" s="1"/>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
       <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
@@ -2697,8 +2771,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
-      <c r="A7" s="1"/>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
       <c r="B7" s="1" t="s">
         <v>16</v>
       </c>
@@ -2757,8 +2831,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
-      <c r="A8" s="1"/>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
       <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
@@ -2817,8 +2891,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
-      <c r="A9" s="1"/>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
       <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
@@ -2877,8 +2951,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
-      <c r="A10" s="1"/>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
       <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
@@ -2937,8 +3011,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
-      <c r="A11" s="1"/>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
       <c r="B11" s="1" t="s">
         <v>20</v>
       </c>
@@ -2997,8 +3071,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
-      <c r="A12" s="1"/>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
       <c r="B12" s="1" t="s">
         <v>21</v>
       </c>
@@ -3057,8 +3131,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
-      <c r="A13" s="1"/>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
       <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
@@ -3117,8 +3191,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
-      <c r="A14" s="1"/>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
       <c r="B14" s="1" t="s">
         <v>23</v>
       </c>
@@ -3177,8 +3251,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
-      <c r="A15" s="1"/>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
       <c r="B15" s="1" t="s">
         <v>24</v>
       </c>
@@ -3237,7 +3311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -3299,8 +3373,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:20">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -3361,8 +3435,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:20">
-      <c r="A18" s="1"/>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
       <c r="B18" s="1" t="s">
         <v>27</v>
       </c>
@@ -3421,8 +3495,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:20">
-      <c r="A19" s="1"/>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
       <c r="B19" s="1" t="s">
         <v>28</v>
       </c>
@@ -3483,12 +3557,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A17:A19"/>
     <mergeCell ref="C1:T1"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:J2"/>
     <mergeCell ref="K2:T2"/>
     <mergeCell ref="A5:A15"/>
-    <mergeCell ref="A17:A19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Dept Risk: Format tab by coll
It was by AIP, but made by collection (and by format name not format version) to scale for large numbers of versions and AIPs.
</commit_message>
<xml_diff>
--- a/documentation/example_dept_report/test_risk_report_202311.xlsx
+++ b/documentation/example_dept_report/test_risk_report_202311.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amhan\Documents\GitHub\format-report\documentation\example_dept_report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriane Hanson\OneDrive - University of Georgia\Documents\GitHub\format-report\documentation\example_dept_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29ECD2E2-434E-4EF4-A17D-63690F07B034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="AIP_Risk_Data" sheetId="1" r:id="rId1"/>
@@ -19,12 +18,15 @@
     <sheet name="AIP_Risk_Levels" sheetId="4" r:id="rId4"/>
     <sheet name="Formats" sheetId="5" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">AIP_Risk_Data!$A$1:$J$40</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="90">
   <si>
     <t>Group</t>
   </si>
@@ -248,9 +250,6 @@
     <t>Comma-Separated Values (CSV) (No Match)</t>
   </si>
   <si>
-    <t>Office Open XML Document 2007 onwards (No Match)</t>
-  </si>
-  <si>
     <t>Office Open XML Workbook (No Match)</t>
   </si>
   <si>
@@ -263,39 +262,12 @@
     <t>Macromedia Flash data, version 5 (Moderate Risk)</t>
   </si>
   <si>
-    <t>PDF/A 1a (Moderate Risk)</t>
-  </si>
-  <si>
     <t>XLSX (Moderate Risk)</t>
   </si>
   <si>
-    <t>Cascading Style Sheet 1 (Low Risk)</t>
-  </si>
-  <si>
-    <t>Cascading Style Sheet 2 (Low Risk)</t>
-  </si>
-  <si>
-    <t>Cascading Style Sheet 2.1 (Low Risk)</t>
-  </si>
-  <si>
     <t>Comma-Separated Values (CSV) (Low Risk)</t>
   </si>
   <si>
-    <t>Hypertext Markup Language 1.1 (Low Risk)</t>
-  </si>
-  <si>
-    <t>Hypertext Markup Language 3.2 (Low Risk)</t>
-  </si>
-  <si>
-    <t>Hypertext Markup Language 4.01 (Low Risk)</t>
-  </si>
-  <si>
-    <t>Hypertext Markup Language 5.1 (Low Risk)</t>
-  </si>
-  <si>
-    <t>PDF/A 1b (Low Risk)</t>
-  </si>
-  <si>
     <t>Plain text (Low Risk)</t>
   </si>
   <si>
@@ -309,12 +281,27 @@
   </si>
   <si>
     <t>Low_Risk_%</t>
+  </si>
+  <si>
+    <t>Office Open XML Document (No Match)</t>
+  </si>
+  <si>
+    <t>PDF/A (Moderate Risk)</t>
+  </si>
+  <si>
+    <t>Cascading Style Sheet (Low Risk)</t>
+  </si>
+  <si>
+    <t>Hypertext Markup Language (Low Risk)</t>
+  </si>
+  <si>
+    <t>PDF/A (Low Risk)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -378,7 +365,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -386,6 +373,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -406,9 +408,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -446,9 +448,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -483,7 +485,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -518,7 +520,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -691,10 +693,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H55" sqref="H55"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1967,41 +1971,42 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:J40"/>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="F5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="F6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="F7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="F8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="F9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="F10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="F11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="F12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="F13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="F14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="F15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="F16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="F17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="F18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="F19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="F20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="F21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="F22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="F26" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="F28" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="F29" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="F33" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="F36" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="F37" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="F4" r:id="rId3"/>
+    <hyperlink ref="F5" r:id="rId4"/>
+    <hyperlink ref="F6" r:id="rId5"/>
+    <hyperlink ref="F7" r:id="rId6"/>
+    <hyperlink ref="F8" r:id="rId7"/>
+    <hyperlink ref="F9" r:id="rId8"/>
+    <hyperlink ref="F10" r:id="rId9"/>
+    <hyperlink ref="F11" r:id="rId10"/>
+    <hyperlink ref="F12" r:id="rId11"/>
+    <hyperlink ref="F13" r:id="rId12"/>
+    <hyperlink ref="F14" r:id="rId13"/>
+    <hyperlink ref="F15" r:id="rId14"/>
+    <hyperlink ref="F16" r:id="rId15"/>
+    <hyperlink ref="F17" r:id="rId16"/>
+    <hyperlink ref="F18" r:id="rId17"/>
+    <hyperlink ref="F19" r:id="rId18"/>
+    <hyperlink ref="F20" r:id="rId19"/>
+    <hyperlink ref="F21" r:id="rId20"/>
+    <hyperlink ref="F22" r:id="rId21"/>
+    <hyperlink ref="F26" r:id="rId22"/>
+    <hyperlink ref="F28" r:id="rId23"/>
+    <hyperlink ref="F29" r:id="rId24"/>
+    <hyperlink ref="F33" r:id="rId25"/>
+    <hyperlink ref="F36" r:id="rId26"/>
+    <hyperlink ref="F37" r:id="rId27"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2024,16 +2029,16 @@
         <v>71</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2062,7 +2067,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2085,16 +2090,16 @@
         <v>71</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2163,7 +2168,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2186,16 +2191,16 @@
         <v>71</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2504,33 +2509,31 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:T19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="59.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="46.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="39.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="39.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="40.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="39.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="59.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="46.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
       <c r="C1" s="3" t="s">
         <v>3</v>
@@ -2547,114 +2550,86 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="3" t="s">
         <v>64</v>
       </c>
+      <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>63</v>
       </c>
+      <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3" t="s">
-        <v>62</v>
-      </c>
+      <c r="J2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+    </row>
+    <row r="3" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="C3" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="K3" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="L3" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="N3" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>14</v>
+      <c r="B5" t="b">
+        <v>0</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -2663,13 +2638,13 @@
         <v>0</v>
       </c>
       <c r="E5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" t="b">
         <v>0</v>
@@ -2678,49 +2653,33 @@
         <v>0</v>
       </c>
       <c r="J5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5" t="b">
         <v>0</v>
       </c>
       <c r="N5" t="b">
-        <v>1</v>
-      </c>
-      <c r="O5" t="b">
-        <v>0</v>
-      </c>
-      <c r="P5" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q5" t="b">
-        <v>0</v>
-      </c>
-      <c r="R5" t="b">
-        <v>0</v>
-      </c>
-      <c r="S5" t="b">
-        <v>0</v>
-      </c>
-      <c r="T5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="b">
+        <v>0</v>
       </c>
       <c r="C6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
@@ -2735,7 +2694,7 @@
         <v>0</v>
       </c>
       <c r="I6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" t="b">
         <v>0</v>
@@ -2747,40 +2706,24 @@
         <v>0</v>
       </c>
       <c r="M6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6" t="b">
         <v>1</v>
       </c>
-      <c r="O6" t="b">
-        <v>0</v>
-      </c>
-      <c r="P6" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R6" t="b">
-        <v>0</v>
-      </c>
-      <c r="S6" t="b">
-        <v>0</v>
-      </c>
-      <c r="T6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="1" t="s">
-        <v>16</v>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="b">
+        <v>1</v>
       </c>
       <c r="C7" t="b">
         <v>0</v>
       </c>
       <c r="D7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
@@ -2792,16 +2735,16 @@
         <v>0</v>
       </c>
       <c r="H7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" t="b">
         <v>0</v>
       </c>
       <c r="K7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7" t="b">
         <v>0</v>
@@ -2812,758 +2755,21 @@
       <c r="N7" t="b">
         <v>1</v>
       </c>
-      <c r="O7" t="b">
-        <v>0</v>
-      </c>
-      <c r="P7" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q7" t="b">
-        <v>0</v>
-      </c>
-      <c r="R7" t="b">
-        <v>0</v>
-      </c>
-      <c r="S7" t="b">
-        <v>0</v>
-      </c>
-      <c r="T7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" t="b">
-        <v>0</v>
-      </c>
-      <c r="F8" t="b">
-        <v>0</v>
-      </c>
-      <c r="G8" t="b">
-        <v>0</v>
-      </c>
-      <c r="H8" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" t="b">
-        <v>0</v>
-      </c>
-      <c r="J8" t="b">
-        <v>0</v>
-      </c>
-      <c r="K8" t="b">
-        <v>0</v>
-      </c>
-      <c r="L8" t="b">
-        <v>0</v>
-      </c>
-      <c r="M8" t="b">
-        <v>0</v>
-      </c>
-      <c r="N8" t="b">
-        <v>1</v>
-      </c>
-      <c r="O8" t="b">
-        <v>0</v>
-      </c>
-      <c r="P8" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q8" t="b">
-        <v>0</v>
-      </c>
-      <c r="R8" t="b">
-        <v>0</v>
-      </c>
-      <c r="S8" t="b">
-        <v>0</v>
-      </c>
-      <c r="T8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" t="b">
-        <v>0</v>
-      </c>
-      <c r="F9" t="b">
-        <v>0</v>
-      </c>
-      <c r="G9" t="b">
-        <v>0</v>
-      </c>
-      <c r="H9" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" t="b">
-        <v>0</v>
-      </c>
-      <c r="J9" t="b">
-        <v>0</v>
-      </c>
-      <c r="K9" t="b">
-        <v>0</v>
-      </c>
-      <c r="L9" t="b">
-        <v>0</v>
-      </c>
-      <c r="M9" t="b">
-        <v>0</v>
-      </c>
-      <c r="N9" t="b">
-        <v>1</v>
-      </c>
-      <c r="O9" t="b">
-        <v>0</v>
-      </c>
-      <c r="P9" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q9" t="b">
-        <v>0</v>
-      </c>
-      <c r="R9" t="b">
-        <v>0</v>
-      </c>
-      <c r="S9" t="b">
-        <v>0</v>
-      </c>
-      <c r="T9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E10" t="b">
-        <v>0</v>
-      </c>
-      <c r="F10" t="b">
-        <v>0</v>
-      </c>
-      <c r="G10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H10" t="b">
-        <v>0</v>
-      </c>
-      <c r="I10" t="b">
-        <v>0</v>
-      </c>
-      <c r="J10" t="b">
-        <v>0</v>
-      </c>
-      <c r="K10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L10" t="b">
-        <v>0</v>
-      </c>
-      <c r="M10" t="b">
-        <v>0</v>
-      </c>
-      <c r="N10" t="b">
-        <v>1</v>
-      </c>
-      <c r="O10" t="b">
-        <v>0</v>
-      </c>
-      <c r="P10" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q10" t="b">
-        <v>0</v>
-      </c>
-      <c r="R10" t="b">
-        <v>0</v>
-      </c>
-      <c r="S10" t="b">
-        <v>0</v>
-      </c>
-      <c r="T10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" t="b">
-        <v>0</v>
-      </c>
-      <c r="D11" t="b">
-        <v>0</v>
-      </c>
-      <c r="E11" t="b">
-        <v>0</v>
-      </c>
-      <c r="F11" t="b">
-        <v>0</v>
-      </c>
-      <c r="G11" t="b">
-        <v>0</v>
-      </c>
-      <c r="H11" t="b">
-        <v>0</v>
-      </c>
-      <c r="I11" t="b">
-        <v>0</v>
-      </c>
-      <c r="J11" t="b">
-        <v>0</v>
-      </c>
-      <c r="K11" t="b">
-        <v>0</v>
-      </c>
-      <c r="L11" t="b">
-        <v>0</v>
-      </c>
-      <c r="M11" t="b">
-        <v>0</v>
-      </c>
-      <c r="N11" t="b">
-        <v>1</v>
-      </c>
-      <c r="O11" t="b">
-        <v>0</v>
-      </c>
-      <c r="P11" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q11" t="b">
-        <v>0</v>
-      </c>
-      <c r="R11" t="b">
-        <v>0</v>
-      </c>
-      <c r="S11" t="b">
-        <v>0</v>
-      </c>
-      <c r="T11" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" t="b">
-        <v>0</v>
-      </c>
-      <c r="D12" t="b">
-        <v>0</v>
-      </c>
-      <c r="E12" t="b">
-        <v>0</v>
-      </c>
-      <c r="F12" t="b">
-        <v>0</v>
-      </c>
-      <c r="G12" t="b">
-        <v>0</v>
-      </c>
-      <c r="H12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I12" t="b">
-        <v>0</v>
-      </c>
-      <c r="J12" t="b">
-        <v>0</v>
-      </c>
-      <c r="K12" t="b">
-        <v>0</v>
-      </c>
-      <c r="L12" t="b">
-        <v>0</v>
-      </c>
-      <c r="M12" t="b">
-        <v>0</v>
-      </c>
-      <c r="N12" t="b">
-        <v>1</v>
-      </c>
-      <c r="O12" t="b">
-        <v>0</v>
-      </c>
-      <c r="P12" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q12" t="b">
-        <v>0</v>
-      </c>
-      <c r="R12" t="b">
-        <v>0</v>
-      </c>
-      <c r="S12" t="b">
-        <v>0</v>
-      </c>
-      <c r="T12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" t="b">
-        <v>0</v>
-      </c>
-      <c r="D13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E13" t="b">
-        <v>0</v>
-      </c>
-      <c r="F13" t="b">
-        <v>0</v>
-      </c>
-      <c r="G13" t="b">
-        <v>0</v>
-      </c>
-      <c r="H13" t="b">
-        <v>0</v>
-      </c>
-      <c r="I13" t="b">
-        <v>0</v>
-      </c>
-      <c r="J13" t="b">
-        <v>0</v>
-      </c>
-      <c r="K13" t="b">
-        <v>0</v>
-      </c>
-      <c r="L13" t="b">
-        <v>0</v>
-      </c>
-      <c r="M13" t="b">
-        <v>0</v>
-      </c>
-      <c r="N13" t="b">
-        <v>1</v>
-      </c>
-      <c r="O13" t="b">
-        <v>0</v>
-      </c>
-      <c r="P13" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q13" t="b">
-        <v>0</v>
-      </c>
-      <c r="R13" t="b">
-        <v>0</v>
-      </c>
-      <c r="S13" t="b">
-        <v>0</v>
-      </c>
-      <c r="T13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" t="b">
-        <v>0</v>
-      </c>
-      <c r="D14" t="b">
-        <v>0</v>
-      </c>
-      <c r="E14" t="b">
-        <v>0</v>
-      </c>
-      <c r="F14" t="b">
-        <v>0</v>
-      </c>
-      <c r="G14" t="b">
-        <v>0</v>
-      </c>
-      <c r="H14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I14" t="b">
-        <v>0</v>
-      </c>
-      <c r="J14" t="b">
-        <v>0</v>
-      </c>
-      <c r="K14" t="b">
-        <v>0</v>
-      </c>
-      <c r="L14" t="b">
-        <v>0</v>
-      </c>
-      <c r="M14" t="b">
-        <v>0</v>
-      </c>
-      <c r="N14" t="b">
-        <v>1</v>
-      </c>
-      <c r="O14" t="b">
-        <v>0</v>
-      </c>
-      <c r="P14" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q14" t="b">
-        <v>0</v>
-      </c>
-      <c r="R14" t="b">
-        <v>0</v>
-      </c>
-      <c r="S14" t="b">
-        <v>0</v>
-      </c>
-      <c r="T14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" t="b">
-        <v>0</v>
-      </c>
-      <c r="D15" t="b">
-        <v>0</v>
-      </c>
-      <c r="E15" t="b">
-        <v>0</v>
-      </c>
-      <c r="F15" t="b">
-        <v>1</v>
-      </c>
-      <c r="G15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J15" t="b">
-        <v>0</v>
-      </c>
-      <c r="K15" t="b">
-        <v>1</v>
-      </c>
-      <c r="L15" t="b">
-        <v>1</v>
-      </c>
-      <c r="M15" t="b">
-        <v>1</v>
-      </c>
-      <c r="N15" t="b">
-        <v>0</v>
-      </c>
-      <c r="O15" t="b">
-        <v>1</v>
-      </c>
-      <c r="P15" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q15" t="b">
-        <v>1</v>
-      </c>
-      <c r="R15" t="b">
-        <v>1</v>
-      </c>
-      <c r="S15" t="b">
-        <v>0</v>
-      </c>
-      <c r="T15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" t="b">
-        <v>1</v>
-      </c>
-      <c r="E16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F16" t="b">
-        <v>0</v>
-      </c>
-      <c r="G16" t="b">
-        <v>0</v>
-      </c>
-      <c r="H16" t="b">
-        <v>0</v>
-      </c>
-      <c r="I16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J16" t="b">
-        <v>1</v>
-      </c>
-      <c r="K16" t="b">
-        <v>0</v>
-      </c>
-      <c r="L16" t="b">
-        <v>0</v>
-      </c>
-      <c r="M16" t="b">
-        <v>0</v>
-      </c>
-      <c r="N16" t="b">
-        <v>0</v>
-      </c>
-      <c r="O16" t="b">
-        <v>0</v>
-      </c>
-      <c r="P16" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q16" t="b">
-        <v>0</v>
-      </c>
-      <c r="R16" t="b">
-        <v>0</v>
-      </c>
-      <c r="S16" t="b">
-        <v>1</v>
-      </c>
-      <c r="T16" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" t="b">
-        <v>1</v>
-      </c>
-      <c r="D17" t="b">
-        <v>0</v>
-      </c>
-      <c r="E17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F17" t="b">
-        <v>0</v>
-      </c>
-      <c r="G17" t="b">
-        <v>0</v>
-      </c>
-      <c r="H17" t="b">
-        <v>0</v>
-      </c>
-      <c r="I17" t="b">
-        <v>0</v>
-      </c>
-      <c r="J17" t="b">
-        <v>1</v>
-      </c>
-      <c r="K17" t="b">
-        <v>0</v>
-      </c>
-      <c r="L17" t="b">
-        <v>0</v>
-      </c>
-      <c r="M17" t="b">
-        <v>0</v>
-      </c>
-      <c r="N17" t="b">
-        <v>1</v>
-      </c>
-      <c r="O17" t="b">
-        <v>0</v>
-      </c>
-      <c r="P17" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q17" t="b">
-        <v>0</v>
-      </c>
-      <c r="R17" t="b">
-        <v>0</v>
-      </c>
-      <c r="S17" t="b">
-        <v>0</v>
-      </c>
-      <c r="T17" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" t="b">
-        <v>0</v>
-      </c>
-      <c r="D18" t="b">
-        <v>0</v>
-      </c>
-      <c r="E18" t="b">
-        <v>1</v>
-      </c>
-      <c r="F18" t="b">
-        <v>0</v>
-      </c>
-      <c r="G18" t="b">
-        <v>0</v>
-      </c>
-      <c r="H18" t="b">
-        <v>0</v>
-      </c>
-      <c r="I18" t="b">
-        <v>1</v>
-      </c>
-      <c r="J18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K18" t="b">
-        <v>0</v>
-      </c>
-      <c r="L18" t="b">
-        <v>0</v>
-      </c>
-      <c r="M18" t="b">
-        <v>0</v>
-      </c>
-      <c r="N18" t="b">
-        <v>0</v>
-      </c>
-      <c r="O18" t="b">
-        <v>0</v>
-      </c>
-      <c r="P18" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q18" t="b">
-        <v>0</v>
-      </c>
-      <c r="R18" t="b">
-        <v>0</v>
-      </c>
-      <c r="S18" t="b">
-        <v>0</v>
-      </c>
-      <c r="T18" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" t="b">
-        <v>1</v>
-      </c>
-      <c r="D19" t="b">
-        <v>0</v>
-      </c>
-      <c r="E19" t="b">
-        <v>1</v>
-      </c>
-      <c r="F19" t="b">
-        <v>0</v>
-      </c>
-      <c r="G19" t="b">
-        <v>0</v>
-      </c>
-      <c r="H19" t="b">
-        <v>0</v>
-      </c>
-      <c r="I19" t="b">
-        <v>0</v>
-      </c>
-      <c r="J19" t="b">
-        <v>1</v>
-      </c>
-      <c r="K19" t="b">
-        <v>0</v>
-      </c>
-      <c r="L19" t="b">
-        <v>0</v>
-      </c>
-      <c r="M19" t="b">
-        <v>0</v>
-      </c>
-      <c r="N19" t="b">
-        <v>1</v>
-      </c>
-      <c r="O19" t="b">
-        <v>0</v>
-      </c>
-      <c r="P19" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q19" t="b">
-        <v>0</v>
-      </c>
-      <c r="R19" t="b">
-        <v>0</v>
-      </c>
-      <c r="S19" t="b">
-        <v>0</v>
-      </c>
-      <c r="T19" t="b">
-        <v>1</v>
-      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="C1:T1"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="K2:T2"/>
-    <mergeCell ref="A5:A15"/>
+  <mergeCells count="4">
+    <mergeCell ref="C1:O1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="J2:N2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>